<commit_message>
assets: update demos and templates
</commit_message>
<xml_diff>
--- a/src/assets/templates/minidyn/PV Minidyn Demo Time - FR.xlsx
+++ b/src/assets/templates/minidyn/PV Minidyn Demo Time - FR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b21a0883c8b69009/Documents/Git/rapportxls/Template Mapview 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spellevrault\Documents\Git\rapportxls\Template Mapview 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FFFEFDA2-A455-40E8-8F33-2297D4B47280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DC90D01-24CA-4257-A992-712B68BC8FD5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC206F6-212C-4985-808E-404C7EA8F1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14230" yWindow="2700" windowWidth="21650" windowHeight="16620" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="3670" windowWidth="28800" windowHeight="15370" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,11 +21,7 @@
     <sheet name="Pi_PointModel" sheetId="27" r:id="rId6"/>
     <sheet name="ImplantationModel" sheetId="15" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="Logo">INDIRECT(VLOOKUP([1]Rapport!$H$2,[1]cache!$A$1:$B$18,2,0))</definedName>
     <definedName name="MapsImage" localSheetId="6">ImplantationModel!$B$17:$I$49</definedName>
     <definedName name="Page" localSheetId="6">ImplantationModel!$J$51</definedName>
     <definedName name="Page" localSheetId="1">PageGardeAModel!$O$49</definedName>
@@ -1673,6 +1669,93 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1688,9 +1771,6 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1719,110 +1799,46 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="23" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="23" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="9" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1835,24 +1851,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1870,9 +1872,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1881,9 +1880,6 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -8646,78 +8642,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Rapport"/>
-      <sheetName val="Feuille de données"/>
-      <sheetName val="cache"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="H2" t="str">
-            <v>GRACCHUS Montpellier</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>MALET</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>cache!$C$1</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Logo</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>cache!$C$4</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>GRACCHUS TLS</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>cache!$C$7</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>GRACCHUS Montpellier</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>cache!$C$10</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>GRACCHUS Bordeaux</v>
-          </cell>
-          <cell r="B13" t="str">
-            <v>cache!$C$13</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>GRACCHUS Lyon</v>
-          </cell>
-          <cell r="B16" t="str">
-            <v>cache!$C$16</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{665143B0-4209-4633-91CB-7C25C94243A4}" name="ArrayPDGBResult" displayName="ArrayPDGBResult" ref="L5:M295" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="L5:M295" xr:uid="{665143B0-4209-4633-91CB-7C25C94243A4}"/>
@@ -9138,7 +9062,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="70" zoomScaleNormal="115" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:P2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -9177,20 +9101,20 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="242" t="s">
+      <c r="E2" s="209" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="243"/>
-      <c r="G2" s="243"/>
-      <c r="H2" s="243"/>
-      <c r="I2" s="243"/>
-      <c r="J2" s="243"/>
-      <c r="K2" s="243"/>
-      <c r="L2" s="243"/>
-      <c r="M2" s="243"/>
-      <c r="N2" s="243"/>
-      <c r="O2" s="243"/>
-      <c r="P2" s="243"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
+      <c r="H2" s="210"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="210"/>
+      <c r="K2" s="210"/>
+      <c r="L2" s="210"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="210"/>
+      <c r="P2" s="210"/>
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -9200,15 +9124,15 @@
       <c r="D3" s="2"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
-      <c r="G3" s="207"/>
-      <c r="H3" s="207"/>
-      <c r="I3" s="207"/>
-      <c r="J3" s="207"/>
-      <c r="K3" s="207"/>
-      <c r="L3" s="207"/>
-      <c r="M3" s="207"/>
-      <c r="N3" s="207"/>
-      <c r="O3" s="207"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
+      <c r="K3" s="211"/>
+      <c r="L3" s="211"/>
+      <c r="M3" s="211"/>
+      <c r="N3" s="211"/>
+      <c r="O3" s="211"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
@@ -9233,9 +9157,9 @@
     </row>
     <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="244"/>
-      <c r="C5" s="244"/>
-      <c r="D5" s="244"/>
+      <c r="B5" s="212"/>
+      <c r="C5" s="212"/>
+      <c r="D5" s="212"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -9252,11 +9176,11 @@
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="245" t="s">
+      <c r="B6" s="213" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="217"/>
-      <c r="D6" s="217"/>
+      <c r="C6" s="214"/>
+      <c r="D6" s="214"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -9272,12 +9196,12 @@
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="246"/>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
+      <c r="A7" s="215"/>
+      <c r="B7" s="215"/>
+      <c r="C7" s="215"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="215"/>
+      <c r="F7" s="215"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
@@ -9291,20 +9215,20 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="247"/>
-      <c r="B8" s="247"/>
-      <c r="C8" s="247"/>
-      <c r="D8" s="247"/>
-      <c r="E8" s="247"/>
-      <c r="F8" s="247"/>
+      <c r="A8" s="216"/>
+      <c r="B8" s="216"/>
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="216"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="248"/>
-      <c r="L8" s="248"/>
-      <c r="M8" s="248"/>
-      <c r="N8" s="248"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="217"/>
+      <c r="M8" s="217"/>
+      <c r="N8" s="217"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -9312,102 +9236,102 @@
     <row r="9" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="27"/>
       <c r="B9" s="28"/>
-      <c r="C9" s="206" t="s">
+      <c r="C9" s="235" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="206"/>
-      <c r="E9" s="206"/>
-      <c r="F9" s="206"/>
-      <c r="G9" s="206"/>
-      <c r="H9" s="206"/>
-      <c r="I9" s="206"/>
-      <c r="J9" s="206"/>
-      <c r="K9" s="206"/>
-      <c r="L9" s="206"/>
-      <c r="M9" s="206"/>
-      <c r="N9" s="206"/>
-      <c r="O9" s="206"/>
+      <c r="D9" s="235"/>
+      <c r="E9" s="235"/>
+      <c r="F9" s="235"/>
+      <c r="G9" s="235"/>
+      <c r="H9" s="235"/>
+      <c r="I9" s="235"/>
+      <c r="J9" s="235"/>
+      <c r="K9" s="235"/>
+      <c r="L9" s="235"/>
+      <c r="M9" s="235"/>
+      <c r="N9" s="235"/>
+      <c r="O9" s="235"/>
       <c r="P9" s="28"/>
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="29"/>
-      <c r="C10" s="207" t="s">
+      <c r="C10" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="207"/>
-      <c r="E10" s="207"/>
-      <c r="F10" s="207"/>
-      <c r="G10" s="207"/>
-      <c r="H10" s="207"/>
-      <c r="I10" s="207"/>
-      <c r="J10" s="207"/>
-      <c r="K10" s="207"/>
-      <c r="L10" s="207"/>
-      <c r="M10" s="207"/>
-      <c r="N10" s="207"/>
-      <c r="O10" s="207"/>
+      <c r="D10" s="211"/>
+      <c r="E10" s="211"/>
+      <c r="F10" s="211"/>
+      <c r="G10" s="211"/>
+      <c r="H10" s="211"/>
+      <c r="I10" s="211"/>
+      <c r="J10" s="211"/>
+      <c r="K10" s="211"/>
+      <c r="L10" s="211"/>
+      <c r="M10" s="211"/>
+      <c r="N10" s="211"/>
+      <c r="O10" s="211"/>
       <c r="P10" s="29"/>
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
       <c r="B11" s="30"/>
-      <c r="C11" s="207"/>
-      <c r="D11" s="207"/>
-      <c r="E11" s="207"/>
-      <c r="F11" s="207"/>
-      <c r="G11" s="207"/>
-      <c r="H11" s="207"/>
-      <c r="I11" s="207"/>
-      <c r="J11" s="207"/>
-      <c r="K11" s="207"/>
-      <c r="L11" s="207"/>
-      <c r="M11" s="207"/>
-      <c r="N11" s="207"/>
-      <c r="O11" s="207"/>
+      <c r="C11" s="211"/>
+      <c r="D11" s="211"/>
+      <c r="E11" s="211"/>
+      <c r="F11" s="211"/>
+      <c r="G11" s="211"/>
+      <c r="H11" s="211"/>
+      <c r="I11" s="211"/>
+      <c r="J11" s="211"/>
+      <c r="K11" s="211"/>
+      <c r="L11" s="211"/>
+      <c r="M11" s="211"/>
+      <c r="N11" s="211"/>
+      <c r="O11" s="211"/>
       <c r="P11" s="30"/>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27"/>
-      <c r="B12" s="240"/>
-      <c r="C12" s="240"/>
-      <c r="D12" s="240"/>
-      <c r="E12" s="240"/>
-      <c r="F12" s="240"/>
-      <c r="G12" s="240"/>
-      <c r="H12" s="240"/>
-      <c r="I12" s="240"/>
-      <c r="J12" s="240"/>
-      <c r="K12" s="240"/>
-      <c r="L12" s="240"/>
-      <c r="M12" s="240"/>
-      <c r="N12" s="240"/>
-      <c r="O12" s="240"/>
-      <c r="P12" s="240"/>
+      <c r="B12" s="202"/>
+      <c r="C12" s="202"/>
+      <c r="D12" s="202"/>
+      <c r="E12" s="202"/>
+      <c r="F12" s="202"/>
+      <c r="G12" s="202"/>
+      <c r="H12" s="202"/>
+      <c r="I12" s="202"/>
+      <c r="J12" s="202"/>
+      <c r="K12" s="202"/>
+      <c r="L12" s="202"/>
+      <c r="M12" s="202"/>
+      <c r="N12" s="202"/>
+      <c r="O12" s="202"/>
+      <c r="P12" s="202"/>
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31"/>
-      <c r="B13" s="226" t="s">
+      <c r="B13" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="227"/>
-      <c r="D13" s="227"/>
-      <c r="E13" s="227"/>
-      <c r="F13" s="227"/>
-      <c r="G13" s="227"/>
-      <c r="H13" s="227"/>
-      <c r="I13" s="227"/>
-      <c r="J13" s="227"/>
-      <c r="K13" s="227"/>
-      <c r="L13" s="227"/>
-      <c r="M13" s="227"/>
-      <c r="N13" s="227"/>
-      <c r="O13" s="227"/>
-      <c r="P13" s="228"/>
+      <c r="C13" s="204"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="204"/>
+      <c r="F13" s="204"/>
+      <c r="G13" s="204"/>
+      <c r="H13" s="204"/>
+      <c r="I13" s="204"/>
+      <c r="J13" s="204"/>
+      <c r="K13" s="204"/>
+      <c r="L13" s="204"/>
+      <c r="M13" s="204"/>
+      <c r="N13" s="204"/>
+      <c r="O13" s="204"/>
+      <c r="P13" s="205"/>
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9417,26 +9341,26 @@
       <c r="D14" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="234" t="e">
+      <c r="E14" s="206" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F14" s="234"/>
-      <c r="G14" s="234"/>
-      <c r="H14" s="234"/>
+      <c r="F14" s="206"/>
+      <c r="G14" s="206"/>
+      <c r="H14" s="206"/>
       <c r="I14" s="103"/>
       <c r="J14" s="103"/>
       <c r="K14" s="103"/>
       <c r="L14" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="220">
+      <c r="M14" s="207">
         <f ca="1">TODAY()</f>
-        <v>44969</v>
-      </c>
-      <c r="N14" s="220"/>
-      <c r="O14" s="220"/>
-      <c r="P14" s="241"/>
+        <v>44991</v>
+      </c>
+      <c r="N14" s="207"/>
+      <c r="O14" s="207"/>
+      <c r="P14" s="208"/>
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9446,26 +9370,26 @@
       <c r="D15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="223" t="e">
+      <c r="E15" s="218" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F15" s="223"/>
-      <c r="G15" s="223"/>
-      <c r="H15" s="223"/>
+      <c r="F15" s="218"/>
+      <c r="G15" s="218"/>
+      <c r="H15" s="218"/>
       <c r="I15" s="101"/>
       <c r="J15" s="101"/>
       <c r="K15" s="73"/>
       <c r="L15" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="M15" s="235" t="e">
+      <c r="M15" s="219" t="e">
         <f>IF(Report_Date="","",Report_Date)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N15" s="235"/>
-      <c r="O15" s="235"/>
-      <c r="P15" s="236"/>
+      <c r="N15" s="219"/>
+      <c r="O15" s="219"/>
+      <c r="P15" s="220"/>
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9475,26 +9399,26 @@
       <c r="D16" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="230" t="e">
+      <c r="E16" s="221" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F16" s="230"/>
-      <c r="G16" s="230"/>
-      <c r="H16" s="230"/>
+      <c r="F16" s="221"/>
+      <c r="G16" s="221"/>
+      <c r="H16" s="221"/>
       <c r="I16" s="107"/>
       <c r="J16" s="107"/>
       <c r="K16" s="107"/>
       <c r="L16" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="232" t="e">
+      <c r="M16" s="222" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N16" s="232"/>
-      <c r="O16" s="232"/>
-      <c r="P16" s="233"/>
+      <c r="N16" s="222"/>
+      <c r="O16" s="222"/>
+      <c r="P16" s="223"/>
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9518,23 +9442,23 @@
     </row>
     <row r="18" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A18" s="36"/>
-      <c r="B18" s="226" t="s">
+      <c r="B18" s="203" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="227"/>
-      <c r="D18" s="227"/>
-      <c r="E18" s="227"/>
-      <c r="F18" s="227"/>
-      <c r="G18" s="227"/>
-      <c r="H18" s="227"/>
-      <c r="I18" s="227"/>
-      <c r="J18" s="227"/>
-      <c r="K18" s="227"/>
-      <c r="L18" s="227"/>
-      <c r="M18" s="227"/>
-      <c r="N18" s="227"/>
-      <c r="O18" s="227"/>
-      <c r="P18" s="228"/>
+      <c r="C18" s="204"/>
+      <c r="D18" s="204"/>
+      <c r="E18" s="204"/>
+      <c r="F18" s="204"/>
+      <c r="G18" s="204"/>
+      <c r="H18" s="204"/>
+      <c r="I18" s="204"/>
+      <c r="J18" s="204"/>
+      <c r="K18" s="204"/>
+      <c r="L18" s="204"/>
+      <c r="M18" s="204"/>
+      <c r="N18" s="204"/>
+      <c r="O18" s="204"/>
+      <c r="P18" s="205"/>
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9544,21 +9468,21 @@
       <c r="D19" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="234" t="e">
+      <c r="E19" s="206" t="e">
         <f>IF(Project_Site="","",Project_Site)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F19" s="234"/>
-      <c r="G19" s="234"/>
-      <c r="H19" s="234"/>
+      <c r="F19" s="206"/>
+      <c r="G19" s="206"/>
+      <c r="H19" s="206"/>
       <c r="I19" s="103"/>
       <c r="J19" s="103"/>
       <c r="K19" s="103"/>
       <c r="L19" s="69"/>
-      <c r="M19" s="220"/>
-      <c r="N19" s="234"/>
-      <c r="O19" s="234"/>
-      <c r="P19" s="237"/>
+      <c r="M19" s="207"/>
+      <c r="N19" s="206"/>
+      <c r="O19" s="206"/>
+      <c r="P19" s="224"/>
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9568,12 +9492,12 @@
       <c r="D20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="223" t="e">
+      <c r="E20" s="218" t="e">
         <f>IF(Report_Lane="","",Report_Lane)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F20" s="223"/>
-      <c r="G20" s="223"/>
+      <c r="F20" s="218"/>
+      <c r="G20" s="218"/>
       <c r="H20" s="104"/>
       <c r="I20" s="104"/>
       <c r="J20" s="104"/>
@@ -9581,13 +9505,13 @@
       <c r="L20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M20" s="238" t="e" cm="1">
+      <c r="M20" s="225" t="e" cm="1">
         <f t="array" ref="M20">IF(Report_Part="","",Report_Part)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N20" s="229"/>
-      <c r="O20" s="229"/>
-      <c r="P20" s="239"/>
+      <c r="N20" s="226"/>
+      <c r="O20" s="226"/>
+      <c r="P20" s="227"/>
       <c r="Q20" s="39"/>
     </row>
     <row r="21" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9597,21 +9521,21 @@
       <c r="D21" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="230" t="e">
+      <c r="E21" s="221" t="e">
         <f>IF(Report_Direction="","",Report_Direction)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F21" s="230"/>
-      <c r="G21" s="230"/>
-      <c r="H21" s="230"/>
+      <c r="F21" s="221"/>
+      <c r="G21" s="221"/>
+      <c r="H21" s="221"/>
       <c r="I21" s="107"/>
       <c r="J21" s="107"/>
       <c r="K21" s="107"/>
       <c r="L21" s="70"/>
-      <c r="M21" s="232"/>
-      <c r="N21" s="232"/>
-      <c r="O21" s="232"/>
-      <c r="P21" s="233"/>
+      <c r="M21" s="222"/>
+      <c r="N21" s="222"/>
+      <c r="O21" s="222"/>
+      <c r="P21" s="223"/>
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9635,23 +9559,23 @@
     </row>
     <row r="23" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A23" s="36"/>
-      <c r="B23" s="226" t="s">
+      <c r="B23" s="203" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="227"/>
-      <c r="D23" s="227"/>
-      <c r="E23" s="227"/>
-      <c r="F23" s="227"/>
-      <c r="G23" s="227"/>
-      <c r="H23" s="227"/>
-      <c r="I23" s="227"/>
-      <c r="J23" s="227"/>
-      <c r="K23" s="227"/>
-      <c r="L23" s="227"/>
-      <c r="M23" s="227"/>
-      <c r="N23" s="227"/>
-      <c r="O23" s="227"/>
-      <c r="P23" s="228"/>
+      <c r="C23" s="204"/>
+      <c r="D23" s="204"/>
+      <c r="E23" s="204"/>
+      <c r="F23" s="204"/>
+      <c r="G23" s="204"/>
+      <c r="H23" s="204"/>
+      <c r="I23" s="204"/>
+      <c r="J23" s="204"/>
+      <c r="K23" s="204"/>
+      <c r="L23" s="204"/>
+      <c r="M23" s="204"/>
+      <c r="N23" s="204"/>
+      <c r="O23" s="204"/>
+      <c r="P23" s="205"/>
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9661,26 +9585,26 @@
       <c r="D24" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="234" t="e">
+      <c r="E24" s="206" t="e">
         <f>IF(Platform_Type="","",Platform_Type)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F24" s="234"/>
-      <c r="G24" s="234"/>
-      <c r="H24" s="234"/>
+      <c r="F24" s="206"/>
+      <c r="G24" s="206"/>
+      <c r="H24" s="206"/>
       <c r="I24" s="103"/>
       <c r="J24" s="103"/>
       <c r="K24" s="103"/>
       <c r="L24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="208" t="e">
+      <c r="M24" s="236" t="e">
         <f>IF(Platform_Layer="","",Platform_Layer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N24" s="208"/>
-      <c r="O24" s="208"/>
-      <c r="P24" s="209"/>
+      <c r="N24" s="236"/>
+      <c r="O24" s="236"/>
+      <c r="P24" s="237"/>
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9690,26 +9614,26 @@
       <c r="D25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="229" t="e">
+      <c r="E25" s="226" t="e">
         <f>IF(Platform_Material="","",Platform_Material)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F25" s="229"/>
-      <c r="G25" s="229"/>
-      <c r="H25" s="229"/>
+      <c r="F25" s="226"/>
+      <c r="G25" s="226"/>
+      <c r="H25" s="226"/>
       <c r="I25" s="104"/>
       <c r="J25" s="104"/>
       <c r="K25" s="104"/>
       <c r="L25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="223" t="e">
+      <c r="M25" s="218" t="e">
         <f>IF(Report_Weather="","",Report_Weather)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N25" s="223"/>
-      <c r="O25" s="223"/>
-      <c r="P25" s="225"/>
+      <c r="N25" s="218"/>
+      <c r="O25" s="218"/>
+      <c r="P25" s="229"/>
       <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9719,26 +9643,26 @@
       <c r="D26" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="230" t="e">
+      <c r="E26" s="221" t="e">
         <f>IF(Platform_Support="","",Platform_Support)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F26" s="231"/>
-      <c r="G26" s="231"/>
-      <c r="H26" s="231"/>
+      <c r="F26" s="230"/>
+      <c r="G26" s="230"/>
+      <c r="H26" s="230"/>
       <c r="I26" s="107"/>
       <c r="J26" s="107"/>
       <c r="K26" s="107"/>
       <c r="L26" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="M26" s="232" t="e">
+      <c r="M26" s="222" t="e">
         <f>IF(Report_Temperature="","",Report_Temperature)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N26" s="232"/>
-      <c r="O26" s="232"/>
-      <c r="P26" s="233"/>
+      <c r="N26" s="222"/>
+      <c r="O26" s="222"/>
+      <c r="P26" s="223"/>
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9762,23 +9686,23 @@
     </row>
     <row r="28" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36"/>
-      <c r="B28" s="226" t="s">
+      <c r="B28" s="203" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="227"/>
-      <c r="D28" s="227"/>
-      <c r="E28" s="227"/>
-      <c r="F28" s="227"/>
-      <c r="G28" s="227"/>
-      <c r="H28" s="227"/>
-      <c r="I28" s="227"/>
-      <c r="J28" s="227"/>
-      <c r="K28" s="227"/>
-      <c r="L28" s="227"/>
-      <c r="M28" s="227"/>
-      <c r="N28" s="227"/>
-      <c r="O28" s="227"/>
-      <c r="P28" s="228"/>
+      <c r="C28" s="204"/>
+      <c r="D28" s="204"/>
+      <c r="E28" s="204"/>
+      <c r="F28" s="204"/>
+      <c r="G28" s="204"/>
+      <c r="H28" s="204"/>
+      <c r="I28" s="204"/>
+      <c r="J28" s="204"/>
+      <c r="K28" s="204"/>
+      <c r="L28" s="204"/>
+      <c r="M28" s="204"/>
+      <c r="N28" s="204"/>
+      <c r="O28" s="204"/>
+      <c r="P28" s="205"/>
       <c r="Q28" s="2"/>
     </row>
     <row r="29" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9788,26 +9712,26 @@
       <c r="D29" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="220" t="e">
+      <c r="E29" s="207" t="e">
         <f xml:space="preserve"> IF(Hardware_SerialNumber="","","Maxidyn " &amp; Hardware_SerialNumber)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F29" s="220"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
+      <c r="F29" s="207"/>
+      <c r="G29" s="207"/>
+      <c r="H29" s="207"/>
       <c r="I29" s="99"/>
       <c r="J29" s="99"/>
       <c r="K29" s="99"/>
       <c r="L29" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="M29" s="221" t="e">
+      <c r="M29" s="247" t="e">
         <f>IF(Hardware_CertificateStart="","",Hardware_CertificateStart)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N29" s="221"/>
-      <c r="O29" s="221"/>
-      <c r="P29" s="222"/>
+      <c r="N29" s="247"/>
+      <c r="O29" s="247"/>
+      <c r="P29" s="248"/>
       <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9817,21 +9741,21 @@
       <c r="D30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="223" t="e" cm="1">
+      <c r="E30" s="218" t="e" cm="1">
         <f t="array" ref="E30">Unit_Modulus_Min &amp;" à " &amp; Unit_Modulus_Max &amp; " MPa"</f>
         <v>#NAME?</v>
       </c>
-      <c r="F30" s="223"/>
-      <c r="G30" s="223"/>
-      <c r="H30" s="224"/>
-      <c r="I30" s="224"/>
-      <c r="J30" s="224"/>
-      <c r="K30" s="224"/>
-      <c r="L30" s="224"/>
-      <c r="M30" s="223"/>
-      <c r="N30" s="223"/>
-      <c r="O30" s="223"/>
-      <c r="P30" s="225"/>
+      <c r="F30" s="218"/>
+      <c r="G30" s="218"/>
+      <c r="H30" s="228"/>
+      <c r="I30" s="228"/>
+      <c r="J30" s="228"/>
+      <c r="K30" s="228"/>
+      <c r="L30" s="228"/>
+      <c r="M30" s="218"/>
+      <c r="N30" s="218"/>
+      <c r="O30" s="218"/>
+      <c r="P30" s="229"/>
       <c r="Q30" s="39"/>
     </row>
     <row r="31" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9855,23 +9779,23 @@
     </row>
     <row r="32" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A32" s="38"/>
-      <c r="B32" s="226" t="s">
+      <c r="B32" s="203" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="227"/>
-      <c r="D32" s="227"/>
-      <c r="E32" s="227"/>
-      <c r="F32" s="227"/>
-      <c r="G32" s="227"/>
-      <c r="H32" s="227"/>
-      <c r="I32" s="227"/>
-      <c r="J32" s="227"/>
-      <c r="K32" s="227"/>
-      <c r="L32" s="227"/>
-      <c r="M32" s="227"/>
-      <c r="N32" s="227"/>
-      <c r="O32" s="227"/>
-      <c r="P32" s="228"/>
+      <c r="C32" s="204"/>
+      <c r="D32" s="204"/>
+      <c r="E32" s="204"/>
+      <c r="F32" s="204"/>
+      <c r="G32" s="204"/>
+      <c r="H32" s="204"/>
+      <c r="I32" s="204"/>
+      <c r="J32" s="204"/>
+      <c r="K32" s="204"/>
+      <c r="L32" s="204"/>
+      <c r="M32" s="204"/>
+      <c r="N32" s="204"/>
+      <c r="O32" s="204"/>
+      <c r="P32" s="205"/>
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -10122,59 +10046,59 @@
       <c r="D44" s="64"/>
       <c r="E44" s="63"/>
       <c r="F44" s="63"/>
-      <c r="G44" s="210" t="s">
+      <c r="G44" s="238" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="210"/>
-      <c r="I44" s="210"/>
-      <c r="J44" s="210"/>
-      <c r="K44" s="210"/>
+      <c r="H44" s="238"/>
+      <c r="I44" s="238"/>
+      <c r="J44" s="238"/>
+      <c r="K44" s="238"/>
       <c r="L44" s="33"/>
-      <c r="M44" s="211" t="s">
+      <c r="M44" s="239" t="s">
         <v>13</v>
       </c>
-      <c r="N44" s="211"/>
-      <c r="O44" s="211"/>
-      <c r="P44" s="212"/>
+      <c r="N44" s="239"/>
+      <c r="O44" s="239"/>
+      <c r="P44" s="240"/>
       <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
-      <c r="B45" s="213" t="e">
+      <c r="B45" s="241" t="e">
         <f>IF(Report_Comment="","",Report_Comment)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C45" s="214"/>
-      <c r="D45" s="214"/>
-      <c r="E45" s="214"/>
-      <c r="F45" s="214"/>
-      <c r="G45" s="217" t="e">
+      <c r="C45" s="242"/>
+      <c r="D45" s="242"/>
+      <c r="E45" s="242"/>
+      <c r="F45" s="242"/>
+      <c r="G45" s="214" t="e">
         <f>IF(Report_Operator="","",Report_Operator)</f>
         <v>#NAME?</v>
       </c>
-      <c r="H45" s="217"/>
-      <c r="I45" s="217"/>
-      <c r="J45" s="217"/>
-      <c r="K45" s="217"/>
+      <c r="H45" s="214"/>
+      <c r="I45" s="214"/>
+      <c r="J45" s="214"/>
+      <c r="K45" s="214"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="218"/>
-      <c r="N45" s="218"/>
-      <c r="O45" s="218"/>
-      <c r="P45" s="219"/>
+      <c r="M45" s="245"/>
+      <c r="N45" s="245"/>
+      <c r="O45" s="245"/>
+      <c r="P45" s="246"/>
       <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
-      <c r="B46" s="213"/>
-      <c r="C46" s="214"/>
-      <c r="D46" s="214"/>
-      <c r="E46" s="214"/>
-      <c r="F46" s="214"/>
-      <c r="G46" s="217"/>
-      <c r="H46" s="217"/>
-      <c r="I46" s="217"/>
-      <c r="J46" s="217"/>
-      <c r="K46" s="217"/>
+      <c r="B46" s="241"/>
+      <c r="C46" s="242"/>
+      <c r="D46" s="242"/>
+      <c r="E46" s="242"/>
+      <c r="F46" s="242"/>
+      <c r="G46" s="214"/>
+      <c r="H46" s="214"/>
+      <c r="I46" s="214"/>
+      <c r="J46" s="214"/>
+      <c r="K46" s="214"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -10184,11 +10108,11 @@
     </row>
     <row r="47" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
-      <c r="B47" s="215"/>
-      <c r="C47" s="216"/>
-      <c r="D47" s="216"/>
-      <c r="E47" s="216"/>
-      <c r="F47" s="216"/>
+      <c r="B47" s="243"/>
+      <c r="C47" s="244"/>
+      <c r="D47" s="244"/>
+      <c r="E47" s="244"/>
+      <c r="F47" s="244"/>
       <c r="G47" s="66"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
@@ -10225,22 +10149,22 @@
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
-      <c r="E49" s="202" t="s">
+      <c r="E49" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="F49" s="202"/>
-      <c r="G49" s="202"/>
-      <c r="H49" s="202"/>
-      <c r="I49" s="202"/>
-      <c r="J49" s="202"/>
-      <c r="K49" s="202"/>
-      <c r="L49" s="202"/>
-      <c r="M49" s="202"/>
+      <c r="F49" s="231"/>
+      <c r="G49" s="231"/>
+      <c r="H49" s="231"/>
+      <c r="I49" s="231"/>
+      <c r="J49" s="231"/>
+      <c r="K49" s="231"/>
+      <c r="L49" s="231"/>
+      <c r="M49" s="231"/>
       <c r="N49" s="8"/>
-      <c r="O49" s="203" t="s">
+      <c r="O49" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="P49" s="203"/>
+      <c r="P49" s="232"/>
       <c r="Q49" s="2"/>
     </row>
     <row r="50" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -10248,56 +10172,24 @@
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="205" t="s">
+      <c r="E50" s="234" t="s">
         <v>18</v>
       </c>
-      <c r="F50" s="205"/>
-      <c r="G50" s="205"/>
-      <c r="H50" s="205"/>
-      <c r="I50" s="205"/>
-      <c r="J50" s="205"/>
-      <c r="K50" s="205"/>
-      <c r="L50" s="205"/>
-      <c r="M50" s="205"/>
+      <c r="F50" s="234"/>
+      <c r="G50" s="234"/>
+      <c r="H50" s="234"/>
+      <c r="I50" s="234"/>
+      <c r="J50" s="234"/>
+      <c r="K50" s="234"/>
+      <c r="L50" s="234"/>
+      <c r="M50" s="234"/>
       <c r="N50" s="2"/>
-      <c r="O50" s="204"/>
-      <c r="P50" s="204"/>
+      <c r="O50" s="233"/>
+      <c r="P50" s="233"/>
       <c r="Q50" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="B12:P12"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="E2:P2"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="B28:P28"/>
-    <mergeCell ref="M25:P25"/>
     <mergeCell ref="E49:M49"/>
     <mergeCell ref="O49:P50"/>
     <mergeCell ref="E50:M50"/>
@@ -10314,6 +10206,38 @@
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="M29:P29"/>
     <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="B28:P28"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B12:P12"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="K8:N8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{22BC0ECF-B0DB-407E-A9DE-C799A88CBDD6}"/>
@@ -10346,28 +10270,28 @@
       <c r="A1" s="145"/>
       <c r="B1" s="145"/>
       <c r="C1" s="145"/>
-      <c r="D1" s="259" t="s">
+      <c r="D1" s="250" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="259"/>
-      <c r="H1" s="259"/>
-      <c r="I1" s="259"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
       <c r="J1" s="145"/>
     </row>
     <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="145"/>
       <c r="B2" s="145"/>
       <c r="C2" s="145"/>
-      <c r="D2" s="260" t="s">
+      <c r="D2" s="251" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="251"/>
       <c r="J2" s="145"/>
       <c r="L2" s="153" t="e" cm="1">
         <f t="array" ref="L2">Thresholds_Modulus_Value</f>
@@ -10387,11 +10311,11 @@
       <c r="G3" s="145" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="261">
+      <c r="H3" s="252">
         <f ca="1">TODAY()</f>
-        <v>44969</v>
-      </c>
-      <c r="I3" s="262"/>
+        <v>44991</v>
+      </c>
+      <c r="I3" s="253"/>
       <c r="J3" s="145"/>
       <c r="L3" s="153" t="e" cm="1">
         <f t="array" ref="L3">Thresholds_Modulus_Value</f>
@@ -10412,11 +10336,11 @@
       <c r="G4" s="145" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="250" t="e">
+      <c r="H4" s="254" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I4" s="250"/>
+      <c r="I4" s="254"/>
       <c r="J4" s="145"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -10439,16 +10363,16 @@
     </row>
     <row r="6" spans="1:13" s="147" customFormat="1" ht="23" x14ac:dyDescent="0.5">
       <c r="A6" s="146"/>
-      <c r="B6" s="263" t="s">
+      <c r="B6" s="255" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="263"/>
-      <c r="D6" s="263"/>
-      <c r="E6" s="263"/>
-      <c r="F6" s="263"/>
-      <c r="G6" s="263"/>
-      <c r="H6" s="263"/>
-      <c r="I6" s="263"/>
+      <c r="C6" s="255"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
       <c r="J6" s="146"/>
       <c r="L6" s="154" t="s">
         <v>46</v>
@@ -10459,16 +10383,16 @@
     </row>
     <row r="7" spans="1:13" s="147" customFormat="1" ht="20" x14ac:dyDescent="0.4">
       <c r="A7" s="146"/>
-      <c r="B7" s="258" t="s">
+      <c r="B7" s="249" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="258"/>
-      <c r="D7" s="258"/>
-      <c r="E7" s="258"/>
-      <c r="F7" s="258"/>
-      <c r="G7" s="258"/>
-      <c r="H7" s="258"/>
-      <c r="I7" s="258"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="249"/>
+      <c r="H7" s="249"/>
+      <c r="I7" s="249"/>
       <c r="J7" s="146"/>
       <c r="L7" s="154"/>
       <c r="M7" s="154"/>
@@ -10505,20 +10429,20 @@
         <v>0</v>
       </c>
       <c r="C10" s="256"/>
-      <c r="D10" s="251" t="e">
+      <c r="D10" s="257" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E10" s="251"/>
+      <c r="E10" s="257"/>
       <c r="F10" s="256" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="256"/>
-      <c r="H10" s="251" t="e">
+      <c r="H10" s="257" t="e">
         <f>IF(Project_Site="","",Project_Site)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I10" s="251"/>
+      <c r="I10" s="257"/>
       <c r="J10" s="145"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -10527,20 +10451,20 @@
         <v>60</v>
       </c>
       <c r="C11" s="256"/>
-      <c r="D11" s="251" t="e">
+      <c r="D11" s="257" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E11" s="251"/>
+      <c r="E11" s="257"/>
       <c r="F11" s="256" t="s">
         <v>61</v>
       </c>
       <c r="G11" s="256"/>
-      <c r="H11" s="251" t="e">
+      <c r="H11" s="257" t="e">
         <f>IF(Platform_Type="","",Platform_Type)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I11" s="251"/>
+      <c r="I11" s="257"/>
       <c r="J11" s="145"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -10549,20 +10473,20 @@
         <v>62</v>
       </c>
       <c r="C12" s="256"/>
-      <c r="D12" s="251" t="e">
+      <c r="D12" s="257" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E12" s="251"/>
+      <c r="E12" s="257"/>
       <c r="F12" s="256" t="s">
         <v>63</v>
       </c>
       <c r="G12" s="256"/>
-      <c r="H12" s="251" t="e">
+      <c r="H12" s="257" t="e">
         <f>IF(Platform_Support="","",Platform_Support)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I12" s="251"/>
+      <c r="I12" s="257"/>
       <c r="J12" s="145"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -10571,20 +10495,20 @@
         <v>64</v>
       </c>
       <c r="C13" s="256"/>
-      <c r="D13" s="251" t="e">
+      <c r="D13" s="257" t="e">
         <f>IF(Project_Project="","", Project_Project)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E13" s="251"/>
+      <c r="E13" s="257"/>
       <c r="F13" s="256" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="256"/>
-      <c r="H13" s="251" t="e">
+      <c r="H13" s="257" t="e">
         <f>IF(Platform_Material="","",Platform_Material)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I13" s="251"/>
+      <c r="I13" s="257"/>
       <c r="J13" s="145"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -10593,37 +10517,37 @@
         <v>66</v>
       </c>
       <c r="C14" s="256"/>
-      <c r="D14" s="251" t="e">
+      <c r="D14" s="257" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E14" s="251"/>
+      <c r="E14" s="257"/>
       <c r="F14" s="256" t="s">
         <v>1</v>
       </c>
       <c r="G14" s="256"/>
-      <c r="H14" s="257" t="e">
+      <c r="H14" s="258" t="e">
         <f>IF(Report_Date="","",Report_Date)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I14" s="257"/>
+      <c r="I14" s="258"/>
       <c r="J14" s="145"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="145"/>
       <c r="B15" s="256"/>
       <c r="C15" s="256"/>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
+      <c r="D15" s="257"/>
+      <c r="E15" s="257"/>
       <c r="F15" s="256" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="256"/>
-      <c r="H15" s="251" t="e">
+      <c r="H15" s="257" t="e">
         <f xml:space="preserve"> IF(Hardware_SerialNumber="","","Maxidyn " &amp; Hardware_SerialNumber)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I15" s="251"/>
+      <c r="I15" s="257"/>
       <c r="J15" s="145"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -10908,85 +10832,85 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="145"/>
-      <c r="B39" s="250" t="s">
+      <c r="B39" s="254" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="250"/>
-      <c r="D39" s="251" t="e">
+      <c r="C39" s="254"/>
+      <c r="D39" s="257" t="e">
         <f>IF(Platform_Layer="","",Platform_Layer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E39" s="251"/>
-      <c r="F39" s="250" t="s">
+      <c r="E39" s="257"/>
+      <c r="F39" s="254" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="250"/>
-      <c r="H39" s="251" t="e">
+      <c r="G39" s="254"/>
+      <c r="H39" s="257" t="e">
         <f>IF(AVERAGE(Pi_Modulus)&gt;Unit_Modulus_Max,"&gt;"&amp;Unit_Modulus_Max,IF(AVERAGE(Pi_Modulus)&lt;Unit_Modulus_Min,"&lt;"&amp;"Unit_Modulus_Max",ROUND(AVERAGE(Pi_Modulus),0)))</f>
         <v>#NAME?</v>
       </c>
-      <c r="I39" s="251"/>
+      <c r="I39" s="257"/>
       <c r="J39" s="145"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="145"/>
-      <c r="B40" s="250" t="s">
+      <c r="B40" s="254" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="250"/>
-      <c r="D40" s="251" t="e">
+      <c r="C40" s="254"/>
+      <c r="D40" s="257" t="e">
         <f>IF(Thresholds_Modulus_Name="","",Thresholds_Modulus_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E40" s="251"/>
-      <c r="F40" s="250" t="s">
+      <c r="E40" s="257"/>
+      <c r="F40" s="254" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="250"/>
-      <c r="H40" s="251" t="e">
+      <c r="G40" s="254"/>
+      <c r="H40" s="257" t="e">
         <f>MAX(Pi_Number)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I40" s="251"/>
+      <c r="I40" s="257"/>
       <c r="J40" s="145"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="145"/>
-      <c r="B41" s="250" t="s">
+      <c r="B41" s="254" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="250"/>
-      <c r="D41" s="251" t="e">
+      <c r="C41" s="254"/>
+      <c r="D41" s="257" t="e">
         <f>IF(OR(_xlfn.SINGLE(Thresholds_Modulus_Value)="",_xlfn.SINGLE(Thresholds_Modulus_Value)=0),"N.C.",_xlfn.SINGLE(Thresholds_Modulus_Value))</f>
         <v>#NAME?</v>
       </c>
-      <c r="E41" s="251"/>
-      <c r="F41" s="250" t="s">
+      <c r="E41" s="257"/>
+      <c r="F41" s="254" t="s">
         <v>73</v>
       </c>
-      <c r="G41" s="250"/>
-      <c r="H41" s="251" t="e" cm="1">
+      <c r="G41" s="254"/>
+      <c r="H41" s="257" t="e" cm="1">
         <f t="array" ref="H41">COUNTIF(Pi_Modulus, "&gt;" &amp;_xlfn.SINGLE( Thresholds_Modulus_Value))</f>
         <v>#NAME?</v>
       </c>
-      <c r="I41" s="251"/>
+      <c r="I41" s="257"/>
       <c r="J41" s="145"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="145"/>
-      <c r="B42" s="250"/>
-      <c r="C42" s="250"/>
-      <c r="D42" s="251"/>
-      <c r="E42" s="251"/>
-      <c r="F42" s="250" t="s">
+      <c r="B42" s="254"/>
+      <c r="C42" s="254"/>
+      <c r="D42" s="257"/>
+      <c r="E42" s="257"/>
+      <c r="F42" s="254" t="s">
         <v>74</v>
       </c>
-      <c r="G42" s="250"/>
-      <c r="H42" s="252" t="e">
+      <c r="G42" s="254"/>
+      <c r="H42" s="260" t="e">
         <f>H41/H40</f>
         <v>#NAME?</v>
       </c>
-      <c r="I42" s="252"/>
+      <c r="I42" s="260"/>
       <c r="J42" s="145"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -11031,48 +10955,48 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="145"/>
-      <c r="B46" s="253" t="e">
+      <c r="B46" s="261" t="e">
         <f>IF(Report_Comment="","",Report_Comment)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C46" s="253"/>
-      <c r="D46" s="253"/>
+      <c r="C46" s="261"/>
+      <c r="D46" s="261"/>
       <c r="E46" s="145"/>
-      <c r="F46" s="254" t="s">
+      <c r="F46" s="262" t="s">
         <v>77</v>
       </c>
-      <c r="G46" s="254"/>
-      <c r="H46" s="254" t="s">
+      <c r="G46" s="262"/>
+      <c r="H46" s="262" t="s">
         <v>78</v>
       </c>
-      <c r="I46" s="254"/>
+      <c r="I46" s="262"/>
       <c r="J46" s="145"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="145"/>
-      <c r="B47" s="253"/>
-      <c r="C47" s="253"/>
-      <c r="D47" s="253"/>
+      <c r="B47" s="261"/>
+      <c r="C47" s="261"/>
+      <c r="D47" s="261"/>
       <c r="E47" s="145"/>
-      <c r="F47" s="255" t="e">
+      <c r="F47" s="263" t="e">
         <f>IF(Report_Operator="","",Report_Operator)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G47" s="255"/>
-      <c r="H47" s="254"/>
-      <c r="I47" s="254"/>
+      <c r="G47" s="263"/>
+      <c r="H47" s="262"/>
+      <c r="I47" s="262"/>
       <c r="J47" s="145"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="145"/>
-      <c r="B48" s="253"/>
-      <c r="C48" s="253"/>
-      <c r="D48" s="253"/>
+      <c r="B48" s="261"/>
+      <c r="C48" s="261"/>
+      <c r="D48" s="261"/>
       <c r="E48" s="145"/>
-      <c r="F48" s="255"/>
-      <c r="G48" s="255"/>
-      <c r="H48" s="254"/>
-      <c r="I48" s="254"/>
+      <c r="F48" s="263"/>
+      <c r="G48" s="263"/>
+      <c r="H48" s="262"/>
+      <c r="I48" s="262"/>
       <c r="J48" s="145"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -11109,10 +11033,10 @@
       <c r="E51" s="145"/>
       <c r="F51" s="145"/>
       <c r="G51" s="145"/>
-      <c r="H51" s="249" t="s">
+      <c r="H51" s="259" t="s">
         <v>8</v>
       </c>
-      <c r="I51" s="249"/>
+      <c r="I51" s="259"/>
       <c r="J51" s="145"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -11143,44 +11067,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D41:E41"/>
@@ -11195,6 +11081,44 @@
     <mergeCell ref="H46:I46"/>
     <mergeCell ref="F47:G48"/>
     <mergeCell ref="H47:I48"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B6:I6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11242,15 +11166,15 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="273" t="s">
+      <c r="D2" s="264" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="273"/>
-      <c r="F2" s="273"/>
-      <c r="G2" s="273"/>
-      <c r="H2" s="273"/>
-      <c r="I2" s="273"/>
-      <c r="J2" s="273"/>
+      <c r="E2" s="264"/>
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="264"/>
+      <c r="I2" s="264"/>
+      <c r="J2" s="264"/>
       <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -11283,49 +11207,49 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="243" t="s">
+      <c r="D5" s="210" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="243"/>
-      <c r="I5" s="243"/>
-      <c r="J5" s="243"/>
-      <c r="K5" s="243"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="210"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="210"/>
+      <c r="J5" s="210"/>
+      <c r="K5" s="210"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="269"/>
-      <c r="B6" s="269"/>
-      <c r="C6" s="269"/>
-      <c r="D6" s="207" t="s">
+      <c r="A6" s="265"/>
+      <c r="B6" s="265"/>
+      <c r="C6" s="265"/>
+      <c r="D6" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="207"/>
-      <c r="F6" s="207"/>
-      <c r="G6" s="207"/>
-      <c r="H6" s="207"/>
-      <c r="I6" s="207"/>
-      <c r="J6" s="207"/>
-      <c r="K6" s="207"/>
+      <c r="E6" s="211"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="211"/>
+      <c r="H6" s="211"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="211"/>
+      <c r="K6" s="211"/>
     </row>
     <row r="7" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="269"/>
-      <c r="B7" s="269"/>
-      <c r="C7" s="269"/>
-      <c r="D7" s="207"/>
-      <c r="E7" s="207"/>
-      <c r="F7" s="207"/>
-      <c r="G7" s="207"/>
-      <c r="H7" s="207"/>
-      <c r="I7" s="207"/>
-      <c r="J7" s="207"/>
-      <c r="K7" s="207"/>
+      <c r="A7" s="265"/>
+      <c r="B7" s="265"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="211"/>
+      <c r="I7" s="211"/>
+      <c r="J7" s="211"/>
+      <c r="K7" s="211"/>
     </row>
     <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="269"/>
-      <c r="B8" s="269"/>
-      <c r="C8" s="269"/>
+      <c r="A8" s="265"/>
+      <c r="B8" s="265"/>
+      <c r="C8" s="265"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -11336,9 +11260,9 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="269"/>
-      <c r="B9" s="269"/>
-      <c r="C9" s="269"/>
+      <c r="A9" s="265"/>
+      <c r="B9" s="265"/>
+      <c r="C9" s="265"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
@@ -11350,17 +11274,17 @@
     </row>
     <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="266" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
-      <c r="H10" s="265"/>
-      <c r="I10" s="265"/>
-      <c r="J10" s="266"/>
+      <c r="C10" s="267"/>
+      <c r="D10" s="267"/>
+      <c r="E10" s="267"/>
+      <c r="F10" s="267"/>
+      <c r="G10" s="267"/>
+      <c r="H10" s="267"/>
+      <c r="I10" s="267"/>
+      <c r="J10" s="268"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11369,11 +11293,11 @@
       <c r="C11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="270" t="e">
+      <c r="D11" s="271" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E11" s="270"/>
+      <c r="E11" s="271"/>
       <c r="F11" s="157"/>
       <c r="G11" s="157"/>
       <c r="H11" s="157"/>
@@ -11382,7 +11306,7 @@
       </c>
       <c r="J11" s="71">
         <f ca="1">TODAY()</f>
-        <v>44969</v>
+        <v>44991</v>
       </c>
       <c r="K11" s="19"/>
     </row>
@@ -11392,11 +11316,11 @@
       <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="271" t="e">
+      <c r="D12" s="272" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E12" s="271"/>
+      <c r="E12" s="272"/>
       <c r="F12" s="158"/>
       <c r="G12" s="158"/>
       <c r="H12" s="158"/>
@@ -11415,11 +11339,11 @@
       <c r="C13" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="272" t="e">
+      <c r="D13" s="273" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E13" s="272"/>
+      <c r="E13" s="273"/>
       <c r="F13" s="160"/>
       <c r="G13" s="160"/>
       <c r="H13" s="160"/>
@@ -11447,17 +11371,17 @@
     </row>
     <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
-      <c r="B15" s="264" t="s">
+      <c r="B15" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="265"/>
-      <c r="D15" s="265"/>
-      <c r="E15" s="265"/>
-      <c r="F15" s="265"/>
-      <c r="G15" s="265"/>
-      <c r="H15" s="265"/>
-      <c r="I15" s="265"/>
-      <c r="J15" s="266"/>
+      <c r="C15" s="267"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
+      <c r="F15" s="267"/>
+      <c r="G15" s="267"/>
+      <c r="H15" s="267"/>
+      <c r="I15" s="267"/>
+      <c r="J15" s="268"/>
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11496,10 +11420,10 @@
       <c r="H17" s="164" t="s">
         <v>89</v>
       </c>
-      <c r="I17" s="267" t="s">
+      <c r="I17" s="269" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="268"/>
+      <c r="J17" s="270"/>
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
@@ -12056,12 +11980,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D5:K5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:K7"/>
     <mergeCell ref="B15:J15"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="A8:C8"/>
@@ -12070,6 +11988,12 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D5:K5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:K6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:K7"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.22058823529411764" bottom="0.40441176470588236" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12118,15 +12042,15 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="242" t="s">
+      <c r="D2" s="209" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
-      <c r="G2" s="242"/>
-      <c r="H2" s="242"/>
-      <c r="I2" s="242"/>
-      <c r="J2" s="242"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
+      <c r="G2" s="209"/>
+      <c r="H2" s="209"/>
+      <c r="I2" s="209"/>
+      <c r="J2" s="209"/>
       <c r="K2" s="76"/>
     </row>
     <row r="3" spans="1:14" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -12159,49 +12083,49 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="243" t="s">
+      <c r="D5" s="210" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="243"/>
-      <c r="I5" s="243"/>
-      <c r="J5" s="243"/>
-      <c r="K5" s="243"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="210"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="210"/>
+      <c r="J5" s="210"/>
+      <c r="K5" s="210"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="269"/>
-      <c r="B6" s="269"/>
-      <c r="C6" s="269"/>
-      <c r="D6" s="207" t="s">
+      <c r="A6" s="265"/>
+      <c r="B6" s="265"/>
+      <c r="C6" s="265"/>
+      <c r="D6" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="207"/>
-      <c r="F6" s="207"/>
-      <c r="G6" s="207"/>
-      <c r="H6" s="207"/>
-      <c r="I6" s="207"/>
-      <c r="J6" s="207"/>
-      <c r="K6" s="207"/>
+      <c r="E6" s="211"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="211"/>
+      <c r="H6" s="211"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="211"/>
+      <c r="K6" s="211"/>
     </row>
     <row r="7" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="269"/>
-      <c r="B7" s="269"/>
-      <c r="C7" s="269"/>
-      <c r="D7" s="207"/>
-      <c r="E7" s="207"/>
-      <c r="F7" s="207"/>
-      <c r="G7" s="207"/>
-      <c r="H7" s="207"/>
-      <c r="I7" s="207"/>
-      <c r="J7" s="207"/>
-      <c r="K7" s="207"/>
+      <c r="A7" s="265"/>
+      <c r="B7" s="265"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="211"/>
+      <c r="I7" s="211"/>
+      <c r="J7" s="211"/>
+      <c r="K7" s="211"/>
     </row>
     <row r="8" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="269"/>
-      <c r="B8" s="269"/>
-      <c r="C8" s="269"/>
+      <c r="A8" s="265"/>
+      <c r="B8" s="265"/>
+      <c r="C8" s="265"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -12212,9 +12136,9 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="269"/>
-      <c r="B9" s="269"/>
-      <c r="C9" s="269"/>
+      <c r="A9" s="265"/>
+      <c r="B9" s="265"/>
+      <c r="C9" s="265"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
@@ -12226,17 +12150,17 @@
     </row>
     <row r="10" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="266" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
-      <c r="H10" s="265"/>
-      <c r="I10" s="265"/>
-      <c r="J10" s="266"/>
+      <c r="C10" s="267"/>
+      <c r="D10" s="267"/>
+      <c r="E10" s="267"/>
+      <c r="F10" s="267"/>
+      <c r="G10" s="267"/>
+      <c r="H10" s="267"/>
+      <c r="I10" s="267"/>
+      <c r="J10" s="268"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -12245,12 +12169,12 @@
       <c r="C11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="234" t="e">
+      <c r="D11" s="206" t="e">
         <f>IF(Project_Name="","",Project_Name)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E11" s="234"/>
-      <c r="F11" s="234"/>
+      <c r="E11" s="206"/>
+      <c r="F11" s="206"/>
       <c r="G11" s="103"/>
       <c r="H11" s="103"/>
       <c r="I11" s="69" t="s">
@@ -12258,7 +12182,7 @@
       </c>
       <c r="J11" s="71">
         <f ca="1">TODAY()</f>
-        <v>44969</v>
+        <v>44991</v>
       </c>
       <c r="K11" s="77"/>
     </row>
@@ -12268,12 +12192,12 @@
       <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="223" t="e">
+      <c r="D12" s="218" t="e">
         <f>IF(Project_Town="","",Project_Town)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E12" s="223"/>
-      <c r="F12" s="223"/>
+      <c r="E12" s="218"/>
+      <c r="F12" s="218"/>
       <c r="G12" s="101"/>
       <c r="H12" s="101"/>
       <c r="I12" s="108" t="s">
@@ -12291,12 +12215,12 @@
       <c r="C13" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="230" t="e">
+      <c r="D13" s="221" t="e">
         <f>IF(Project_Customer="","",Project_Customer)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E13" s="230"/>
-      <c r="F13" s="230"/>
+      <c r="E13" s="221"/>
+      <c r="F13" s="221"/>
       <c r="G13" s="107"/>
       <c r="H13" s="107"/>
       <c r="I13" s="70" t="s">
@@ -12323,17 +12247,17 @@
     </row>
     <row r="15" spans="1:14" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
-      <c r="B15" s="264" t="s">
+      <c r="B15" s="266" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="265"/>
-      <c r="D15" s="265"/>
-      <c r="E15" s="265"/>
-      <c r="F15" s="265"/>
-      <c r="G15" s="265"/>
-      <c r="H15" s="265"/>
-      <c r="I15" s="265"/>
-      <c r="J15" s="266"/>
+      <c r="C15" s="267"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
+      <c r="F15" s="267"/>
+      <c r="G15" s="267"/>
+      <c r="H15" s="267"/>
+      <c r="I15" s="267"/>
+      <c r="J15" s="268"/>
       <c r="K15" s="15"/>
       <c r="L15" s="80"/>
       <c r="M15" s="80"/>
@@ -12933,6 +12857,39 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D5:K5"/>
@@ -12945,39 +12902,6 @@
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="G45:J45"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.22058823529411764" bottom="0.40441176470588236" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13020,13 +12944,13 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="242" t="s">
+      <c r="D2" s="209" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
-      <c r="G2" s="242"/>
-      <c r="H2" s="242"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
+      <c r="G2" s="209"/>
+      <c r="H2" s="209"/>
       <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:15" ht="14.15" customHeight="1" x14ac:dyDescent="0.3">
@@ -13055,43 +12979,43 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="243" t="s">
+      <c r="D5" s="210" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="243"/>
-      <c r="I5" s="243"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="210"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="210"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="269"/>
-      <c r="B6" s="269"/>
-      <c r="C6" s="269"/>
-      <c r="D6" s="207" t="s">
+      <c r="A6" s="265"/>
+      <c r="B6" s="265"/>
+      <c r="C6" s="265"/>
+      <c r="D6" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="207"/>
-      <c r="F6" s="207"/>
-      <c r="G6" s="207"/>
-      <c r="H6" s="207"/>
-      <c r="I6" s="207"/>
+      <c r="E6" s="211"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="211"/>
+      <c r="H6" s="211"/>
+      <c r="I6" s="211"/>
     </row>
     <row r="7" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="269"/>
-      <c r="B7" s="269"/>
-      <c r="C7" s="269"/>
-      <c r="D7" s="207"/>
-      <c r="E7" s="207"/>
-      <c r="F7" s="207"/>
-      <c r="G7" s="207"/>
-      <c r="H7" s="207"/>
-      <c r="I7" s="207"/>
+      <c r="A7" s="265"/>
+      <c r="B7" s="265"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="211"/>
+      <c r="I7" s="211"/>
     </row>
     <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="269"/>
-      <c r="B8" s="269"/>
-      <c r="C8" s="269"/>
+      <c r="A8" s="265"/>
+      <c r="B8" s="265"/>
+      <c r="C8" s="265"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -13100,9 +13024,9 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="269"/>
-      <c r="B9" s="269"/>
-      <c r="C9" s="269"/>
+      <c r="A9" s="265"/>
+      <c r="B9" s="265"/>
+      <c r="C9" s="265"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
@@ -13112,15 +13036,15 @@
     </row>
     <row r="10" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="266" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
-      <c r="H10" s="266"/>
+      <c r="C10" s="267"/>
+      <c r="D10" s="267"/>
+      <c r="E10" s="267"/>
+      <c r="F10" s="267"/>
+      <c r="G10" s="267"/>
+      <c r="H10" s="268"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -13140,7 +13064,7 @@
       </c>
       <c r="H11" s="71">
         <f ca="1">TODAY()</f>
-        <v>44969</v>
+        <v>44991</v>
       </c>
       <c r="I11" s="77"/>
     </row>
@@ -13199,16 +13123,16 @@
     </row>
     <row r="15" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
-      <c r="B15" s="264" t="e" cm="1">
+      <c r="B15" s="266" t="e" cm="1">
         <f t="array" ref="B15">"INFORMATIONS DU POINT " &amp; Pi_Number</f>
         <v>#NAME?</v>
       </c>
-      <c r="C15" s="265"/>
-      <c r="D15" s="265"/>
-      <c r="E15" s="265"/>
-      <c r="F15" s="265"/>
-      <c r="G15" s="265"/>
-      <c r="H15" s="266"/>
+      <c r="C15" s="267"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
+      <c r="F15" s="267"/>
+      <c r="G15" s="267"/>
+      <c r="H15" s="268"/>
       <c r="I15" s="15"/>
       <c r="L15" s="80"/>
       <c r="M15" s="80"/>
@@ -16737,7 +16661,7 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" view="pageLayout" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16766,14 +16690,14 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="273" t="s">
+      <c r="D2" s="264" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="273"/>
-      <c r="F2" s="273"/>
-      <c r="G2" s="273"/>
-      <c r="H2" s="273"/>
-      <c r="I2" s="273"/>
+      <c r="E2" s="264"/>
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="264"/>
+      <c r="I2" s="264"/>
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16804,46 +16728,46 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="243" t="s">
+      <c r="D5" s="210" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="243"/>
-      <c r="F5" s="243"/>
-      <c r="G5" s="243"/>
-      <c r="H5" s="243"/>
-      <c r="I5" s="243"/>
-      <c r="J5" s="243"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="210"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="210"/>
+      <c r="J5" s="210"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="269"/>
-      <c r="B6" s="269"/>
-      <c r="C6" s="269"/>
-      <c r="D6" s="207" t="s">
+      <c r="A6" s="265"/>
+      <c r="B6" s="265"/>
+      <c r="C6" s="265"/>
+      <c r="D6" s="211" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="207"/>
-      <c r="F6" s="207"/>
-      <c r="G6" s="207"/>
-      <c r="H6" s="207"/>
-      <c r="I6" s="207"/>
-      <c r="J6" s="207"/>
+      <c r="E6" s="211"/>
+      <c r="F6" s="211"/>
+      <c r="G6" s="211"/>
+      <c r="H6" s="211"/>
+      <c r="I6" s="211"/>
+      <c r="J6" s="211"/>
     </row>
     <row r="7" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="269"/>
-      <c r="B7" s="269"/>
-      <c r="C7" s="269"/>
-      <c r="D7" s="207"/>
-      <c r="E7" s="207"/>
-      <c r="F7" s="207"/>
-      <c r="G7" s="207"/>
-      <c r="H7" s="207"/>
-      <c r="I7" s="207"/>
-      <c r="J7" s="207"/>
+      <c r="A7" s="265"/>
+      <c r="B7" s="265"/>
+      <c r="C7" s="265"/>
+      <c r="D7" s="211"/>
+      <c r="E7" s="211"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="211"/>
+      <c r="I7" s="211"/>
+      <c r="J7" s="211"/>
     </row>
     <row r="8" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="269"/>
-      <c r="B8" s="269"/>
-      <c r="C8" s="269"/>
+      <c r="A8" s="265"/>
+      <c r="B8" s="265"/>
+      <c r="C8" s="265"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -16853,9 +16777,9 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="269"/>
-      <c r="B9" s="269"/>
-      <c r="C9" s="269"/>
+      <c r="A9" s="265"/>
+      <c r="B9" s="265"/>
+      <c r="C9" s="265"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
@@ -16866,16 +16790,16 @@
     </row>
     <row r="10" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="266" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
-      <c r="H10" s="265"/>
-      <c r="I10" s="266"/>
+      <c r="C10" s="267"/>
+      <c r="D10" s="267"/>
+      <c r="E10" s="267"/>
+      <c r="F10" s="267"/>
+      <c r="G10" s="267"/>
+      <c r="H10" s="267"/>
+      <c r="I10" s="268"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -16896,7 +16820,7 @@
       </c>
       <c r="I11" s="22">
         <f ca="1">TODAY()</f>
-        <v>44969</v>
+        <v>44991</v>
       </c>
       <c r="J11" s="19"/>
     </row>
@@ -16958,16 +16882,16 @@
     </row>
     <row r="15" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
-      <c r="B15" s="264" t="s">
+      <c r="B15" s="266" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="265"/>
-      <c r="D15" s="265"/>
-      <c r="E15" s="265"/>
-      <c r="F15" s="265"/>
-      <c r="G15" s="265"/>
-      <c r="H15" s="265"/>
-      <c r="I15" s="266"/>
+      <c r="C15" s="267"/>
+      <c r="D15" s="267"/>
+      <c r="E15" s="267"/>
+      <c r="F15" s="267"/>
+      <c r="G15" s="267"/>
+      <c r="H15" s="267"/>
+      <c r="I15" s="268"/>
       <c r="J15" s="15"/>
       <c r="M15" s="23"/>
       <c r="N15" s="23"/>

</xml_diff>